<commit_message>
Finishing touches to tutorial
I finished writing the tutorial, and fixed a little bug in the visualization and cavity scripts.
</commit_message>
<xml_diff>
--- a/data/test_data.xlsx
+++ b/data/test_data.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26230"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28908"/>
   <workbookPr showInkAnnotation="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robertmarsland/Documents/community-simulator/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robertmarsland/Documents/GitHub/community-simulator/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="2440" yWindow="480" windowWidth="25600" windowHeight="14320" tabRatio="500" activeTab="4"/>
+    <workbookView xWindow="2440" yWindow="480" windowWidth="25600" windowHeight="14320" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Populations" sheetId="1" r:id="rId1"/>
@@ -21,6 +21,9 @@
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -700,8 +703,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -778,7 +781,7 @@
         <v>1E-3</v>
       </c>
       <c r="C3">
-        <v>0.9</v>
+        <v>0.99</v>
       </c>
       <c r="D3">
         <v>0.01</v>
@@ -807,10 +810,10 @@
         <v>10</v>
       </c>
       <c r="B4">
-        <v>0.6</v>
+        <v>0.48</v>
       </c>
       <c r="C4">
-        <v>0.7</v>
+        <v>0.49</v>
       </c>
       <c r="D4">
         <v>0.01</v>
@@ -839,10 +842,10 @@
         <v>11</v>
       </c>
       <c r="B5" s="2">
-        <v>0.7</v>
+        <v>0.49</v>
       </c>
       <c r="C5">
-        <v>0.6</v>
+        <v>0.48</v>
       </c>
       <c r="D5">
         <v>0.01</v>
@@ -942,7 +945,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>

</xml_diff>